<commit_message>
add benchmarks results and graphics
</commit_message>
<xml_diff>
--- a/Task_2_1_1/results/BenchamrksGraphics.xlsx
+++ b/Task_2_1_1/results/BenchamrksGraphics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1\OOP\Task_2_1_1\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1270D5-1341-482B-A333-6CD83206A84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8325C1F-7D8C-44B3-82CC-5FAAC70675C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{9C0B5ECA-F7DF-4B5C-AED9-D2F99EEFD0A3}"/>
   </bookViews>
@@ -709,6 +709,109 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-43B1-425A-B0B7-9DDA75FC1A85}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>ParallelThread(32 Threads)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$B$57:$B$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$E$57:$E$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.3369999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4459999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.6349999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7649999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.5790000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.170999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>74.335999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>143.369</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-43B1-425A-B0B7-9DDA75FC1A85}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3371,8 +3474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14B4A3D-7A5C-4866-8B38-3EB26263F624}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="87" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:A65"/>
+    <sheetView tabSelected="1" topLeftCell="E26" zoomScale="123" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
add another one graphic
</commit_message>
<xml_diff>
--- a/Task_2_1_1/results/BenchamrksGraphics.xlsx
+++ b/Task_2_1_1/results/BenchamrksGraphics.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1\OOP\Task_2_1_1\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8325C1F-7D8C-44B3-82CC-5FAAC70675C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{04F57A4E-2F82-4DAA-B7F8-56D367E95FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{9C0B5ECA-F7DF-4B5C-AED9-D2F99EEFD0A3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="1" xr2:uid="{9C0B5ECA-F7DF-4B5C-AED9-D2F99EEFD0A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="19">
   <si>
     <t>BenchmarkDifferentTypes.Linear</t>
   </si>
@@ -55,6 +56,33 @@
   </si>
   <si>
     <t>BenchmarkDifferentTypes.ParallelThread(32 Threads)</t>
+  </si>
+  <si>
+    <t>Benchmark</t>
+  </si>
+  <si>
+    <t>(threadsCount)</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Cnt</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>BenchmarkThreadsCount.parallelThread</t>
+  </si>
+  <si>
+    <t>BenchmarkDifferentTypes.parallelStream</t>
   </si>
 </sst>
 </file>
@@ -1293,41 +1321,29 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Лист1!$C$28:$C$38</c:f>
+              <c:f>Лист1!$C$32:$C$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
@@ -1335,41 +1351,29 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$E$28:$E$38</c:f>
+              <c:f>Лист1!$E$32:$E$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5545.9480000000003</c:v>
+                  <c:v>907.23699999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3028.0450000000001</c:v>
+                  <c:v>703.37900000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1700.3019999999999</c:v>
+                  <c:v>667.65099999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1193.8720000000001</c:v>
+                  <c:v>667.92899999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>907.23699999999997</c:v>
+                  <c:v>665.16899999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>703.37900000000002</c:v>
+                  <c:v>649.86900000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>667.65099999999995</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>667.92899999999997</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>665.16899999999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>649.86900000000003</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>673.64300000000003</c:v>
                 </c:pt>
               </c:numCache>
@@ -1414,41 +1418,29 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Лист1!$C$28:$C$38</c:f>
+              <c:f>Лист1!$C$32:$C$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
@@ -1456,10 +1448,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$G$28:$G$38</c:f>
+              <c:f>Лист1!$G$32:$G$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>664.95899999999995</c:v>
                 </c:pt>
@@ -1479,18 +1471,6 @@
                   <c:v>664.95899999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>664.95899999999995</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>664.95899999999995</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>664.95899999999995</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>664.95899999999995</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>664.95899999999995</c:v>
                 </c:pt>
               </c:numCache>
@@ -1500,127 +1480,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-38AB-419B-95BF-CDB659FAA7B8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Linear</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Лист1!$C$28:$C$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>50</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Лист1!$H$28:$H$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>5274.3379999999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5274.3379999999997</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5274.3379999999997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5274.3379999999997</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5274.3379999999997</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5274.3379999999997</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5274.3379999999997</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5274.3379999999997</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5274.3379999999997</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5274.3379999999997</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5274.3379999999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-38AB-419B-95BF-CDB659FAA7B8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1634,6 +1493,145 @@
         </c:dLbls>
         <c:axId val="1971689535"/>
         <c:axId val="1971699519"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v>Linear</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Лист1!$C$28:$C$38</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="11"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>40</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>50</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Лист1!$H$28:$H$38</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="11"/>
+                      <c:pt idx="0">
+                        <c:v>5274.3379999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>5274.3379999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>5274.3379999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>5274.3379999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5274.3379999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>5274.3379999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>5274.3379999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>5274.3379999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>5274.3379999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>5274.3379999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>5274.3379999999997</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-38AB-419B-95BF-CDB659FAA7B8}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="1971689535"/>
@@ -1986,6 +1984,567 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.1131648050054568E-2"/>
+          <c:y val="4.960927552134161E-2"/>
+          <c:w val="0.7752630546104754"/>
+          <c:h val="0.86613944643223839"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Threads</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист2!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>512</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист2!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>363.11799999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>311.38299999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>301.43799999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300.76</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300.20999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>305.79300000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>84.084000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>96.391000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>250.447</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-510A-4946-9E59-B28A661EEBC1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Threads variant 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист2!$D$12:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>375.43700000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>317.779</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>307.767</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>308.15199999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>307.77300000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>307.964</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>125.66200000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>182.54400000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>189.31200000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-510A-4946-9E59-B28A661EEBC1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Stream</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист2!$D$22:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>311.15699999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>311.15699999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>311.15699999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>311.15699999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>311.15699999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>311.15699999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>311.15699999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>311.15699999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>311.15699999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-510A-4946-9E59-B28A661EEBC1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Threads var3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист2!$D$32:$D$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>369.37299999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>317.46899999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>304.67700000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>303.81700000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>311.70600000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>312.16500000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>58.767000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>84.322000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>384.28699999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-510A-4946-9E59-B28A661EEBC1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="538114464"/>
+        <c:axId val="538122144"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="538114464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="538122144"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="538122144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="538114464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2066,6 +2625,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3079,6 +3678,509 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -3167,6 +4269,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>73024</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0383314C-37F3-354F-FEF5-E79F99130F94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3474,8 +4617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14B4A3D-7A5C-4866-8B38-3EB26263F624}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E26" zoomScale="123" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView topLeftCell="A46" zoomScale="123" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4848,4 +5991,658 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6876DA2-55E0-46A2-A3B1-EFD0E05EDFAB}">
+  <dimension ref="A1:G40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="42.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>363.11799999999999</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>311.38299999999998</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>301.43799999999999</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>300.76</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>300.20999999999998</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>305.79300000000001</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>128</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>84.084000000000003</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>256</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>96.391000000000005</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>512</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>250.447</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>375.43700000000001</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>317.779</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>307.767</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>308.15199999999999</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>307.77300000000002</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>307.964</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>128</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>125.66200000000001</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>256</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>182.54400000000001</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>512</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>189.31200000000001</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>311.15699999999998</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>311.15699999999998</v>
+      </c>
+      <c r="E23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>311.15699999999998</v>
+      </c>
+      <c r="E24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>311.15699999999998</v>
+      </c>
+      <c r="E25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>311.15699999999998</v>
+      </c>
+      <c r="E26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27">
+        <v>64</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>311.15699999999998</v>
+      </c>
+      <c r="E27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28">
+        <v>128</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>311.15699999999998</v>
+      </c>
+      <c r="E28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29">
+        <v>256</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>311.15699999999998</v>
+      </c>
+      <c r="E29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30">
+        <v>512</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>311.15699999999998</v>
+      </c>
+      <c r="E30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>369.37299999999999</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33">
+        <v>12</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>317.46899999999999</v>
+      </c>
+      <c r="E33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34">
+        <v>16</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>304.67700000000002</v>
+      </c>
+      <c r="E34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35">
+        <v>24</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>303.81700000000001</v>
+      </c>
+      <c r="E35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36">
+        <v>32</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>311.70600000000002</v>
+      </c>
+      <c r="E36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37">
+        <v>64</v>
+      </c>
+      <c r="C37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>312.16500000000002</v>
+      </c>
+      <c r="E37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38">
+        <v>128</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>58.767000000000003</v>
+      </c>
+      <c r="E38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39">
+        <v>256</v>
+      </c>
+      <c r="C39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>84.322000000000003</v>
+      </c>
+      <c r="E39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40">
+        <v>512</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>384.28699999999998</v>
+      </c>
+      <c r="E40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>